<commit_message>
updated requirements file and partA document
</commit_message>
<xml_diff>
--- a/part A/requirements.xlsx
+++ b/part A/requirements.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\obarilan\Documents\University\Analysis-Design\part A\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="140">
   <si>
     <t>תאור הדרישה</t>
   </si>
@@ -437,9 +432,6 @@
     <t>הזמנת קופונים תתאפשר ע"י משתמשים רשומים במערכת.</t>
   </si>
   <si>
-    <t>אורי</t>
-  </si>
-  <si>
     <t>Column1</t>
   </si>
   <si>
@@ -447,87 +439,17 @@
   </si>
   <si>
     <t>Column2</t>
-  </si>
-  <si>
-    <t>פיצול מדהים</t>
-  </si>
-  <si>
-    <t>מדהים</t>
-  </si>
-  <si>
-    <t>מבסוט</t>
-  </si>
-  <si>
-    <t>מותר לנסח מחדש? שלא יתפסו אותנו במילה ש"חייב" זה אימות שהוא לא פונקציונאלי... אם אפשר לנסח מחדש אולי שווה לכתוב משהו כמו "בעת הרשמה למערכת, המערכת תדרוש מהמשתמש העדפה של קטגוריה בלה בלה ....". מה אתם אומרים?</t>
-  </si>
-  <si>
-    <t>נראה לי שכדאי להוסיף במקור 'מנתח מערכת'</t>
-  </si>
-  <si>
-    <r>
-      <t>נראה לי שצריך ל</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>שנות</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> במקור ל'מנתח מערכת'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">לא סגור על זה, משום מה אני זוכר שהיה דיבור ששינוי של מצב פנימי בלבד אומר שזה לא פונקציונלי, למרות שמצד שני זה נשמע מאוד פונקציונלי כי רשום </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>יתעדכן הקופון למצב מומש</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> אז לא יודע...</t>
-    </r>
-  </si>
-  <si>
-    <t>אפשר אולי להשוות בטלפון רק נקודות שאנחנו לא בטוחים בהם עם הקבוצה של נועם או משהו אם עדיין מתלבטים אחרי שכולם עברו על זה שוב</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -536,7 +458,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -544,7 +466,7 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -553,7 +475,7 @@
       <i/>
       <sz val="14"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -561,33 +483,26 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -597,24 +512,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -643,7 +540,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -654,15 +551,14 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="טקסט הסברי" xfId="1" builtinId="53"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
@@ -1082,7 +978,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1092,24 +988,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="C31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="21.875" customWidth="1"/>
+    <col min="3" max="3" width="30.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="154" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" customWidth="1"/>
-    <col min="8" max="8" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.25" customWidth="1"/>
+    <col min="6" max="6" width="28.125" customWidth="1"/>
+    <col min="7" max="7" width="20.875" customWidth="1"/>
+    <col min="8" max="8" width="255.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1132,13 +1028,13 @@
         <v>7</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="18.75">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1149,7 +1045,7 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" ht="70.5" customHeight="1">
+    <row r="3" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>100</v>
       </c>
@@ -1174,7 +1070,7 @@
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:9" ht="18.75">
+    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1185,7 +1081,7 @@
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:9" ht="18.75">
+    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>50</v>
       </c>
@@ -1210,7 +1106,7 @@
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" ht="18.75">
+    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>51</v>
       </c>
@@ -1235,7 +1131,7 @@
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="1:9" ht="18.75">
+    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>52</v>
       </c>
@@ -1260,7 +1156,7 @@
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" ht="18.75">
+    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>53</v>
       </c>
@@ -1285,7 +1181,7 @@
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" ht="18.75">
+    <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>54</v>
       </c>
@@ -1310,7 +1206,7 @@
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="18.75">
+    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>55</v>
       </c>
@@ -1335,7 +1231,7 @@
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9" ht="18.75">
+    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>56</v>
       </c>
@@ -1360,7 +1256,7 @@
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:9" ht="18.75">
+    <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>102</v>
       </c>
@@ -1385,7 +1281,7 @@
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="18.75">
+    <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>103</v>
       </c>
@@ -1410,7 +1306,7 @@
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:9" ht="18.75">
+    <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>106</v>
       </c>
@@ -1435,7 +1331,7 @@
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:9" ht="18.75">
+    <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1446,7 +1342,7 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" ht="18.75">
+    <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>57</v>
       </c>
@@ -1471,7 +1367,7 @@
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="1:9" ht="18.75">
+    <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>58</v>
       </c>
@@ -1496,7 +1392,7 @@
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="1:9" ht="18.75">
+    <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>59</v>
       </c>
@@ -1521,7 +1417,7 @@
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:9" ht="18.75">
+    <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>60</v>
       </c>
@@ -1546,7 +1442,7 @@
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:9" ht="18.75">
+    <row r="20" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>62</v>
       </c>
@@ -1571,7 +1467,7 @@
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" ht="18.75">
+    <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>88</v>
       </c>
@@ -1596,7 +1492,7 @@
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="1:9" ht="18.75">
+    <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>90</v>
       </c>
@@ -1621,7 +1517,7 @@
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="1:9" ht="18.75">
+    <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1632,7 +1528,7 @@
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:9" ht="18.75">
+    <row r="24" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>61</v>
       </c>
@@ -1654,14 +1550,12 @@
       <c r="G24" s="3">
         <v>5</v>
       </c>
-      <c r="H24" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="H24" s="9"/>
       <c r="I24" s="7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="18.75">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>63</v>
       </c>
@@ -1677,19 +1571,17 @@
       <c r="E25" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="10" t="s">
         <v>130</v>
       </c>
       <c r="G25" s="3">
         <v>5</v>
       </c>
-      <c r="H25" s="7" t="s">
-        <v>141</v>
-      </c>
+      <c r="H25" s="9"/>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="1:9" ht="18.75">
-      <c r="A26" s="9" t="s">
+    <row r="26" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>131</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -1701,20 +1593,20 @@
       <c r="D26" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E26" s="7"/>
+      <c r="E26" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="F26" s="7" t="s">
         <v>125</v>
       </c>
       <c r="G26" s="7">
         <v>5</v>
       </c>
-      <c r="H26" s="12" t="s">
-        <v>145</v>
-      </c>
+      <c r="H26" s="9"/>
       <c r="I26" s="7"/>
     </row>
-    <row r="27" spans="1:9" ht="18.75">
-      <c r="A27" s="9" t="s">
+    <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>132</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -1726,19 +1618,19 @@
       <c r="D27" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="E27" s="7"/>
+      <c r="E27" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="F27" s="7" t="s">
         <v>126</v>
       </c>
       <c r="G27" s="7">
         <v>5</v>
       </c>
-      <c r="H27" s="12" t="s">
-        <v>145</v>
-      </c>
+      <c r="H27" s="9"/>
       <c r="I27" s="7"/>
     </row>
-    <row r="28" spans="1:9" ht="18.75">
+    <row r="28" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>64</v>
       </c>
@@ -1760,10 +1652,10 @@
       <c r="G28" s="3">
         <v>5</v>
       </c>
-      <c r="H28" s="7"/>
+      <c r="H28" s="9"/>
       <c r="I28" s="7"/>
     </row>
-    <row r="29" spans="1:9" ht="18.75">
+    <row r="29" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>65</v>
       </c>
@@ -1785,12 +1677,10 @@
       <c r="G29" s="3">
         <v>3</v>
       </c>
-      <c r="H29" s="12" t="s">
-        <v>144</v>
-      </c>
+      <c r="H29" s="9"/>
       <c r="I29" s="7"/>
     </row>
-    <row r="30" spans="1:9" ht="18.75">
+    <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>66</v>
       </c>
@@ -1806,18 +1696,16 @@
       <c r="E30" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="9" t="s">
         <v>125</v>
       </c>
       <c r="G30" s="3">
         <v>5</v>
       </c>
-      <c r="H30" s="7" t="s">
-        <v>142</v>
-      </c>
+      <c r="H30" s="9"/>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="1:9" ht="18.75">
+    <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>67</v>
       </c>
@@ -1839,10 +1727,10 @@
       <c r="G31" s="3">
         <v>3</v>
       </c>
-      <c r="H31" s="7"/>
+      <c r="H31" s="9"/>
       <c r="I31" s="7"/>
     </row>
-    <row r="32" spans="1:9" ht="18.75">
+    <row r="32" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>68</v>
       </c>
@@ -1864,10 +1752,10 @@
       <c r="G32" s="3">
         <v>5</v>
       </c>
-      <c r="H32" s="7"/>
+      <c r="H32" s="9"/>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="1:9" ht="18.75">
+    <row r="33" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>69</v>
       </c>
@@ -1889,10 +1777,10 @@
       <c r="G33" s="3">
         <v>3</v>
       </c>
-      <c r="H33" s="7"/>
+      <c r="H33" s="9"/>
       <c r="I33" s="7"/>
     </row>
-    <row r="34" spans="1:9" ht="18.75">
+    <row r="34" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>70</v>
       </c>
@@ -1914,10 +1802,10 @@
       <c r="G34" s="3">
         <v>4</v>
       </c>
-      <c r="H34" s="7"/>
+      <c r="H34" s="9"/>
       <c r="I34" s="7"/>
     </row>
-    <row r="35" spans="1:9" ht="18.75">
+    <row r="35" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1925,10 +1813,10 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
-      <c r="H35" s="7"/>
+      <c r="H35" s="9"/>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="1:9" ht="18.75">
+    <row r="36" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>71</v>
       </c>
@@ -1950,13 +1838,11 @@
       <c r="G36" s="3">
         <v>5</v>
       </c>
-      <c r="H36" s="7" t="s">
-        <v>141</v>
-      </c>
+      <c r="H36" s="9"/>
       <c r="I36" s="7"/>
     </row>
-    <row r="37" spans="1:9" ht="18.75">
-      <c r="A37" s="9" t="s">
+    <row r="37" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
         <v>133</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -1969,7 +1855,7 @@
         <v>135</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>125</v>
@@ -1977,13 +1863,11 @@
       <c r="G37" s="3">
         <v>5</v>
       </c>
-      <c r="H37" s="12" t="s">
-        <v>146</v>
-      </c>
+      <c r="H37" s="9"/>
       <c r="I37" s="7"/>
     </row>
-    <row r="38" spans="1:9" ht="18.75">
-      <c r="A38" s="9" t="s">
+    <row r="38" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
         <v>134</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -1996,7 +1880,7 @@
         <v>136</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>126</v>
@@ -2004,12 +1888,10 @@
       <c r="G38" s="3">
         <v>5</v>
       </c>
-      <c r="H38" s="12" t="s">
-        <v>146</v>
-      </c>
+      <c r="H38" s="9"/>
       <c r="I38" s="7"/>
     </row>
-    <row r="39" spans="1:9" ht="18.75">
+    <row r="39" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>72</v>
       </c>
@@ -2025,18 +1907,16 @@
       <c r="E39" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F39" s="9" t="s">
         <v>126</v>
       </c>
       <c r="G39" s="3">
         <v>5</v>
       </c>
-      <c r="H39" s="7" t="s">
-        <v>143</v>
-      </c>
+      <c r="H39" s="9"/>
       <c r="I39" s="7"/>
     </row>
-    <row r="40" spans="1:9" ht="18.75">
+    <row r="40" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>73</v>
       </c>
@@ -2058,10 +1938,10 @@
       <c r="G40" s="3">
         <v>4</v>
       </c>
-      <c r="H40" s="7"/>
+      <c r="H40" s="9"/>
       <c r="I40" s="7"/>
     </row>
-    <row r="41" spans="1:9" ht="18.75">
+    <row r="41" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>74</v>
       </c>
@@ -2083,10 +1963,10 @@
       <c r="G41" s="3">
         <v>4</v>
       </c>
-      <c r="H41" s="7"/>
+      <c r="H41" s="9"/>
       <c r="I41" s="7"/>
     </row>
-    <row r="42" spans="1:9" ht="18.75">
+    <row r="42" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>75</v>
       </c>
@@ -2102,18 +1982,16 @@
       <c r="E42" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F42" s="8" t="s">
+      <c r="F42" s="9" t="s">
         <v>125</v>
       </c>
       <c r="G42" s="3">
         <v>4</v>
       </c>
-      <c r="H42" s="7" t="s">
-        <v>143</v>
-      </c>
+      <c r="H42" s="9"/>
       <c r="I42" s="7"/>
     </row>
-    <row r="43" spans="1:9" ht="18.75">
+    <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>110</v>
       </c>
@@ -2129,18 +2007,16 @@
       <c r="E43" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F43" s="10" t="s">
+      <c r="F43" s="9" t="s">
         <v>125</v>
       </c>
       <c r="G43" s="3">
         <v>4</v>
       </c>
-      <c r="H43" s="12" t="s">
-        <v>147</v>
-      </c>
+      <c r="H43" s="9"/>
       <c r="I43" s="7"/>
     </row>
-    <row r="44" spans="1:9" ht="18.75">
+    <row r="44" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>76</v>
       </c>
@@ -2165,7 +2041,7 @@
       <c r="H44" s="7"/>
       <c r="I44" s="7"/>
     </row>
-    <row r="45" spans="1:9" ht="18.75">
+    <row r="45" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>77</v>
       </c>
@@ -2190,7 +2066,7 @@
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
     </row>
-    <row r="46" spans="1:9" ht="18.75">
+    <row r="46" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -2201,7 +2077,7 @@
       <c r="H46" s="7"/>
       <c r="I46" s="7"/>
     </row>
-    <row r="47" spans="1:9" ht="18.75">
+    <row r="47" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>78</v>
       </c>
@@ -2224,7 +2100,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="18.75">
+    <row r="48" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>79</v>
       </c>
@@ -2241,16 +2117,14 @@
         <v>85</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G48" s="3">
         <v>4</v>
       </c>
-      <c r="H48" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="18.75">
+      <c r="H48" s="7"/>
+    </row>
+    <row r="49" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>80</v>
       </c>
@@ -2273,7 +2147,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="18.75">
+    <row r="50" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>113</v>
       </c>
@@ -2296,7 +2170,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="18.75">
+    <row r="51" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>81</v>
       </c>
@@ -2319,7 +2193,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="18.75">
+    <row r="52" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -2328,7 +2202,7 @@
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
     </row>
-    <row r="53" spans="1:7" ht="18.75">
+    <row r="53" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>82</v>
       </c>
@@ -2351,7 +2225,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="18.75">
+    <row r="54" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>83</v>
       </c>
@@ -2374,7 +2248,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="18.75">
+    <row r="55" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>84</v>
       </c>
@@ -2397,7 +2271,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="18.75">
+    <row r="56" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -2406,18 +2280,16 @@
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
     </row>
-    <row r="57" spans="1:7" ht="18.75">
+    <row r="57" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
-      <c r="D57" s="12" t="s">
-        <v>148</v>
-      </c>
+      <c r="D57" s="9"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
     </row>
-    <row r="58" spans="1:7" ht="18.75">
+    <row r="58" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -2426,7 +2298,7 @@
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
     </row>
-    <row r="59" spans="1:7" ht="18.75">
+    <row r="59" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -2435,7 +2307,7 @@
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
     </row>
-    <row r="60" spans="1:7" ht="18.75">
+    <row r="60" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -2444,7 +2316,7 @@
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
     </row>
-    <row r="61" spans="1:7" ht="18.75">
+    <row r="61" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -2453,7 +2325,7 @@
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
     </row>
-    <row r="62" spans="1:7" ht="18.75">
+    <row r="62" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -2462,7 +2334,7 @@
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
     </row>
-    <row r="63" spans="1:7" ht="18.75">
+    <row r="63" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -2471,7 +2343,7 @@
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
     </row>
-    <row r="64" spans="1:7" ht="18.75">
+    <row r="64" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -2480,7 +2352,7 @@
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
     </row>
-    <row r="65" spans="1:7" ht="18.75">
+    <row r="65" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -2489,7 +2361,7 @@
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
     </row>
-    <row r="66" spans="1:7" ht="18.75">
+    <row r="66" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -2498,7 +2370,7 @@
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
     </row>
-    <row r="67" spans="1:7" ht="18.75">
+    <row r="67" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -2507,7 +2379,7 @@
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
     </row>
-    <row r="68" spans="1:7" ht="18.75">
+    <row r="68" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>

</xml_diff>